<commit_message>
Re-worked analyses to be more descriptive
</commit_message>
<xml_diff>
--- a/analysis/NC/NC2022-metrics.xlsx
+++ b/analysis/NC/NC2022-metrics.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/method_eval/analysis/NC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0193F1D-49B9-8F44-8278-D7AA0E42CC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA41CBE-4AF4-6F4C-AA57-6B599C2C56AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10720" yWindow="6280" windowWidth="27260" windowHeight="16940" xr2:uid="{CA548A59-6448-2647-90EB-1CE001C8D079}"/>
+    <workbookView xWindow="12340" yWindow="5180" windowWidth="27260" windowHeight="16940" xr2:uid="{CA548A59-6448-2647-90EB-1CE001C8D079}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All" sheetId="1" r:id="rId1"/>
+    <sheet name="Vf" sheetId="2" r:id="rId2"/>
+    <sheet name="Sf" sheetId="3" r:id="rId3"/>
+    <sheet name="Decl" sheetId="4" r:id="rId4"/>
+    <sheet name="Responsiveness" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="NC2022_metrics" localSheetId="0">Sheet1!$A$1:$L$34</definedName>
+    <definedName name="NC2022_metrics" localSheetId="0">All!$A$1:$L$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="45">
   <si>
     <t>METRIC</t>
   </si>
@@ -206,7 +210,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -222,6 +226,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,7 +250,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -257,11 +276,146 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -275,9 +429,18 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,7 +765,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N7" sqref="N7:O7"/>
+      <selection pane="bottomRight" activeCell="L20" sqref="A1:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -998,43 +1161,42 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="3">
         <v>2.4599999999999999E-3</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="3">
         <v>8.4019999999999997E-3</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="3">
         <v>1.7539999999999999E-3</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="3">
         <v>3.297E-3</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="3">
         <v>-4.4320000000000002E-3</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="3">
         <v>3.7309999999999999E-3</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="3">
         <v>1.8220000000000001E-3</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="3">
         <v>2.4290000000000002E-3</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="3">
         <v>1.6930000000000001E-3</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="3">
         <v>3.1000000000000001E-5</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="3">
         <v>1.8311000000000001E-2</v>
       </c>
-      <c r="M11" s="13"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
@@ -1832,5 +1994,425 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246B81BD-9576-6A4B-9B7D-347A88A9A240}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="12" width="7.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0.49433300000000002</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0.49314400000000003</v>
+      </c>
+      <c r="D2" s="15">
+        <v>0.48094100000000001</v>
+      </c>
+      <c r="E2" s="15">
+        <v>0.49085200000000001</v>
+      </c>
+      <c r="F2" s="15">
+        <v>0.47044399999999997</v>
+      </c>
+      <c r="G2" s="15">
+        <v>0.52287499999999998</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0.50124299999999999</v>
+      </c>
+      <c r="I2" s="15">
+        <v>0.49325000000000002</v>
+      </c>
+      <c r="J2" s="15">
+        <v>7.3460000000000001E-3</v>
+      </c>
+      <c r="K2" s="15">
+        <v>1.083E-3</v>
+      </c>
+      <c r="L2" s="16">
+        <v>0.147427</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662BAFD6-5846-E24B-9398-ED5206259979}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="12" width="7.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0.48244700000000001</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0.47445500000000002</v>
+      </c>
+      <c r="D2" s="15">
+        <v>0.450154</v>
+      </c>
+      <c r="E2" s="15">
+        <v>0.47141300000000003</v>
+      </c>
+      <c r="F2" s="15">
+        <v>0.40962900000000002</v>
+      </c>
+      <c r="G2" s="15">
+        <v>0.56120999999999999</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0.50139199999999995</v>
+      </c>
+      <c r="I2" s="15">
+        <v>0.47804200000000002</v>
+      </c>
+      <c r="J2" s="15">
+        <v>2.0798000000000001E-2</v>
+      </c>
+      <c r="K2" s="15">
+        <v>4.4050000000000001E-3</v>
+      </c>
+      <c r="L2" s="16">
+        <v>0.21179899999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D134AD-2605-844C-8A7D-54B46ABB5DDF}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="9" width="8.83203125" customWidth="1"/>
+    <col min="10" max="12" width="7.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0.18129799999999999</v>
+      </c>
+      <c r="C2" s="15">
+        <v>1.229868</v>
+      </c>
+      <c r="D2" s="15">
+        <v>-2.5586999999999999E-2</v>
+      </c>
+      <c r="E2" s="15">
+        <v>0.29150900000000002</v>
+      </c>
+      <c r="F2" s="15">
+        <v>-0.152085</v>
+      </c>
+      <c r="G2" s="15">
+        <v>6.1559999999999997E-2</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0.161607</v>
+      </c>
+      <c r="I2" s="15">
+        <v>0.26114500000000002</v>
+      </c>
+      <c r="J2" s="15">
+        <v>0.20347499999999999</v>
+      </c>
+      <c r="K2" s="15">
+        <v>-7.9847000000000001E-2</v>
+      </c>
+      <c r="L2" s="16">
+        <v>-0.39241700000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83453B9-E1F2-AE42-AF51-EEF8F5C3046A}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="12" width="7.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="18">
+        <v>3.0973999999999999</v>
+      </c>
+      <c r="C2" s="18">
+        <v>3.7259000000000002</v>
+      </c>
+      <c r="D2" s="18">
+        <v>2.6154000000000002</v>
+      </c>
+      <c r="E2" s="18">
+        <v>3.125</v>
+      </c>
+      <c r="F2" s="18">
+        <v>3.0575999999999999</v>
+      </c>
+      <c r="G2" s="18">
+        <v>2.6758000000000002</v>
+      </c>
+      <c r="H2" s="18">
+        <v>1.1198999999999999</v>
+      </c>
+      <c r="I2" s="18">
+        <v>2.7199</v>
+      </c>
+      <c r="J2" s="18">
+        <v>0.35880000000000001</v>
+      </c>
+      <c r="K2" s="18">
+        <v>0.37740000000000001</v>
+      </c>
+      <c r="L2" s="19">
+        <v>1.0519000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="21">
+        <v>2.6265000000000001</v>
+      </c>
+      <c r="C3" s="21">
+        <v>2.4298999999999999</v>
+      </c>
+      <c r="D3" s="21">
+        <v>2.2683</v>
+      </c>
+      <c r="E3" s="21">
+        <v>2.6499000000000001</v>
+      </c>
+      <c r="F3" s="21">
+        <v>2.8363999999999998</v>
+      </c>
+      <c r="G3" s="21">
+        <v>2.8159999999999998</v>
+      </c>
+      <c r="H3" s="21">
+        <v>2.6312000000000002</v>
+      </c>
+      <c r="I3" s="21">
+        <v>2.6053000000000002</v>
+      </c>
+      <c r="J3" s="21">
+        <v>9.0300000000000005E-2</v>
+      </c>
+      <c r="K3" s="21">
+        <v>2.12E-2</v>
+      </c>
+      <c r="L3" s="22">
+        <v>0.23449999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>